<commit_message>
Napredovanje/izpad ekip iz lige
prikaz ekipa, ki so v določeni sezoni napredovale oz. izpadle iz prve lige
</commit_message>
<xml_diff>
--- a/laliga_all_seasons.xlsx
+++ b/laliga_all_seasons.xlsx
@@ -12,6 +12,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sestevek naslovov" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsota podatkov" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Povprecje zmag in tock" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Napredovanje_izpad" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -43411,4 +43412,640 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Sezona</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Izpadle ekipe</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Napredovane ekipe</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1993-1994</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>{'Lerida', 'Osasuna', 'Rayo Vallecano'}</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>{'Espanyol', 'Real Betis', 'Compostela'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1994-1995</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{'CD Logroñés'}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{'Mérida UD', 'UD Salamanca', 'Rayo Vallecano'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1995-1996</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>{'Albacete', 'Mérida UD', 'UD Salamanca'}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{'CF Extremadura', 'Hércules', 'CD Logroñés'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1996-1997</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>{'CD Logroñés', 'Sevilla', 'Hércules', 'Rayo Vallecano', 'CF Extremadura'}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{'Mérida UD', 'UD Salamanca', 'Mallorca'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1997-1998</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'Mérida UD', 'Sporting Gijon', 'Compostela'}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{'Alaves', 'Villarreal', 'CF Extremadura'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1998-1999</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'Villarreal', 'Tenerife', 'UD Salamanca', 'CF Extremadura'}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>{'Numancia', 'Sevilla', 'Malaga', 'Rayo Vallecano'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1999-2000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'Atletico Madrid', 'Sevilla', 'Real Betis'}</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>{'Las Palmas', 'Villarreal', 'Osasuna'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2000-2001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>{'Numancia', 'Real Oviedo', 'Racing Santander'}</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>{'Sevilla', 'Tenerife', 'Real Betis'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2001-2002</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'Las Palmas', 'Real Zaragoza', 'Tenerife'}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>{'Atletico Madrid', 'Racing Santander', 'Recreativo Huelva'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2002-2003</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'Recreativo Huelva', 'Alaves', 'Rayo Vallecano'}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>{'Real Murcia', 'Albacete', 'Real Zaragoza'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2003-2004</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'Real Murcia', 'Real Valladolid', 'Celta Vigo'}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>{'Numancia', 'Getafe', 'Levante'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2004-2005</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'Albacete', 'Numancia', 'Levante'}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>{'Alaves', 'Cadiz', 'Celta Vigo'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2005-2006</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'Alaves', 'Cadiz', 'Malaga'}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>{'Recreativo Huelva', 'Gimnàstic Tarr…', 'Levante'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2006-2007</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'Gimnàstic Tarr…', 'Real Sociedad', 'Celta Vigo'}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>{'Real Murcia', 'Almeria', 'Real Valladolid'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2007-2008</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'Real Murcia', 'Real Zaragoza', 'Levante'}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>{'Numancia', 'Malaga', 'Sporting Gijon'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2008-2009</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'Recreativo Huelva', 'Numancia', 'Real Betis'}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>{'Xerez', 'Real Zaragoza', 'Tenerife'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2009-2010</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'Xerez', 'Tenerife', 'Real Valladolid'}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>{'Hércules', 'Real Sociedad', 'Levante'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2010-2011</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'Hércules', 'Almeria', 'Deportivo La C…'}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>{'Granada', 'Rayo Vallecano', 'Real Betis'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2011-2012</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'Racing Santander', 'Villarreal', 'Sporting Gijon'}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>{'Celta Vigo', 'Real Valladolid', 'Deportivo La C…'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2012-2013</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'Real Zaragoza', 'Mallorca', 'Deportivo La C…'}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>{'Villarreal', 'Elche', 'Almeria'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2013-2014</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'Osasuna', 'Real Valladolid', 'Real Betis'}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>{'Eibar', 'Córdoba', 'Deportivo La C…'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2014-2015</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'Elche', 'Córdoba', 'Almeria'}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>{'Las Palmas', 'Sporting Gijon', 'Real Betis'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2015-2016</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'Getafe', 'Rayo Vallecano', 'Levante'}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>{'Alaves', 'Leganes', 'Osasuna'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2016-2017</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'Granada', 'Osasuna', 'Sporting Gijon'}</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>{'Levante', 'Getafe', 'Girona'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2017-2018</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'Las Palmas', 'Malaga', 'Deportivo La C…'}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>{'Huesca', 'Rayo Vallecano', 'Real Valladolid'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2018-2019</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'Huesca', 'Rayo Vallecano', 'Girona'}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>{'Granada', 'Osasuna', 'Mallorca'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2019-2020</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'Espanyol', 'Leganes', 'Mallorca'}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>{'Elche', 'Cadiz', 'Huesca'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2020-2021</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'Huesca', 'Real Valladolid', 'Eibar'}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>{'Espanyol', 'Rayo Vallecano', 'Mallorca'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2021-2022</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'Alaves', 'Granada', 'Levante'}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>{'Almeria', 'Real Valladolid', 'Girona'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2022-2023</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'Espanyol', 'Elche', 'Real Valladolid'}</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>{'Las Palmas', 'Granada', 'Alaves'}</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Najvec zadetkov v sezoni
Graf ki prikazuje ekipo z najvec zadetki med letom 1993 in 2023

excel dokument z vsemi rezultati analize in osnovnimi podatki
</commit_message>
<xml_diff>
--- a/laliga_all_seasons.xlsx
+++ b/laliga_all_seasons.xlsx
@@ -13,6 +13,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsota podatkov" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Povprecje zmag in tock" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Napredovanje_izpad" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Najvecd zadetkov po sezonah" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44048,4 +44049,598 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Season</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Goals for</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1993-1994</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1994-1995</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1995-1996</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1996-1997</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1997-1998</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Atletico Madrid</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1998-1999</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1999-2000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2000-2001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2001-2002</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2002-2003</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2003-2004</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2004-2005</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2005-2006</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2006-2007</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2007-2008</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2008-2009</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2009-2010</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2010-2011</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2011-2012</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2012-2013</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2013-2014</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2014-2015</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2015-2016</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2016-2017</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2017-2018</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2018-2019</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2019-2020</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2020-2021</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2021-2022</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2022-2023</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>